<commit_message>
Actualizaciones al modulo de reportes
</commit_message>
<xml_diff>
--- a/Front-SIPROE/public/assets/Asignacion_Directa.xlsx
+++ b/Front-SIPROE/public/assets/Asignacion_Directa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCTOS DEL TRABAJO\253 SIPROE aleatorio\Reporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\SIPROE\Front-SIPROE\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132C6350-69EA-412C-B262-C349D21101BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094D8601-5791-4150-8E73-AEBEA010E5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>SECRETARIA EJECUTIVA</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hora: </t>
-  </si>
-  <si>
-    <t>11:30:45 Hrs.</t>
   </si>
   <si>
     <t>DIRECCIÓN DISTRITAL</t>
@@ -211,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,38 +232,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,27 +618,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="3" max="3" width="36.81640625" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" customWidth="1"/>
-    <col min="6" max="6" width="29.7265625" customWidth="1"/>
-    <col min="7" max="7" width="82.1796875" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="18.1796875" customWidth="1"/>
-    <col min="11" max="11" width="18.453125" customWidth="1"/>
-    <col min="12" max="12" width="27.7265625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="82.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -656,7 +656,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -672,29 +672,29 @@
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H4" s="5"/>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
@@ -710,7 +710,7 @@
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -723,36 +723,34 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="8"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
+      <c r="B9" s="7"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
       <c r="F9" s="1"/>
@@ -763,50 +761,48 @@
         <v>45736</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="20"/>
+    </row>
+    <row r="11" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+      <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="G11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="J11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="K11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="L11" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>